<commit_message>
Modified some Test Cases
</commit_message>
<xml_diff>
--- a/CoverageTest Input.xlsx
+++ b/CoverageTest Input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ionut-mihai.nicula\Documents\UiPath\Produt Ownership\Test-Suite\Studio Pro\RPA_CICD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath.sharepoint.com/sites/Presales/Shared Documents/11. PUBLIC (CREATE PERSONAL FOLDER HERE)/IonutNicula/[Training] AMER PS/0. Exercises/3. RPA/Exercise 3 Solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188FD07D-6007-4F26-87AB-DB170401CC85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{188FD07D-6007-4F26-87AB-DB170401CC85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4AE14351-6E85-426C-A21B-56C755FE114B}"/>
   <bookViews>
     <workbookView xWindow="1185" yWindow="4335" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Documents\Request Form.pdf</t>
   </si>
   <si>
-    <t>Documents\Simple Invoice.pdf</t>
+    <t>files</t>
   </si>
   <si>
-    <t>files</t>
+    <t>Documents\no_classification.pdf</t>
+  </si>
+  <si>
+    <t>Documents\Simple Invoice.pdf</t>
   </si>
 </sst>
 </file>
@@ -869,17 +872,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -889,10 +892,469 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Contributor xmlns="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7" xsi:nil="true"/>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <b53ad4c2841e4e4a94cda0d52ee6ae4c xmlns="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b53ad4c2841e4e4a94cda0d52ee6ae4c>
+    <o8b80352c99244c0ae4e61fbd1c4c1b6 xmlns="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o8b80352c99244c0ae4e61fbd1c4c1b6>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <kc0fc4540b5243a08bdce71e5c11795d xmlns="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </kc0fc4540b5243a08bdce71e5c11795d>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="6eaee64e-3edc-4652-811c-08ca3112fb23"/>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <o967d7aa727040ce921a448a49d7d2c5 xmlns="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </o967d7aa727040ce921a448a49d7d2c5>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B97771E766E7464F8B629707C04FE572" ma:contentTypeVersion="48" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4ef64722d29ea3516173811612e3b54e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7" xmlns:ns3="6eaee64e-3edc-4652-811c-08ca3112fb23" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ec86d8155bebec1b0a7034793984d33" ns1:_="" ns2:_="" ns3:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7"/>
+    <xsd:import namespace="6eaee64e-3edc-4652-811c-08ca3112fb23"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns1:AverageRating" minOccurs="0"/>
+                <xsd:element ref="ns1:RatingCount" minOccurs="0"/>
+                <xsd:element ref="ns1:LikesCount" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:b53ad4c2841e4e4a94cda0d52ee6ae4c" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:o8b80352c99244c0ae4e61fbd1c4c1b6" minOccurs="0"/>
+                <xsd:element ref="ns1:RatedBy" minOccurs="0"/>
+                <xsd:element ref="ns1:Ratings" minOccurs="0"/>
+                <xsd:element ref="ns1:LikedBy" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:o967d7aa727040ce921a448a49d7d2c5" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:kc0fc4540b5243a08bdce71e5c11795d" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:_Flow_SignoffStatus" minOccurs="0"/>
+                <xsd:element ref="ns2:Contributor" minOccurs="0"/>
+                <xsd:element ref="ns1:KpiDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="AverageRating" ma:index="5" nillable="true" ma:displayName="Rating (0-5)" ma:decimals="2" ma:description="Average value of all the ratings that have been submitted" ma:internalName="AverageRating" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RatingCount" ma:index="6" nillable="true" ma:displayName="Number of Ratings" ma:decimals="0" ma:description="Number of ratings submitted" ma:internalName="RatingCount" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Number"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LikesCount" ma:index="7" nillable="true" ma:displayName="Number of Likes" ma:internalName="LikesCount">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="RatedBy" ma:index="18" nillable="true" ma:displayName="Rated By" ma:description="Users rated the item." ma:hidden="true" ma:list="UserInfo" ma:internalName="RatedBy">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Ratings" ma:index="19" nillable="true" ma:displayName="User ratings" ma:description="User ratings for the item" ma:hidden="true" ma:internalName="Ratings">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LikedBy" ma:index="20" nillable="true" ma:displayName="Liked By" ma:hidden="true" ma:list="UserInfo" ma:internalName="LikedBy">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="KpiDescription" ma:index="34" nillable="true" ma:displayName="Description" ma:description="The description provides information about the purpose of the goal." ma:internalName="KpiDescription">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="36" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="37" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="b53ad4c2841e4e4a94cda0d52ee6ae4c" ma:index="14" nillable="true" ma:taxonomy="true" ma:internalName="b53ad4c2841e4e4a94cda0d52ee6ae4c" ma:taxonomyFieldName="Industry" ma:displayName="Industries" ma:default="" ma:fieldId="{b53ad4c2-841e-4e4a-94cd-a0d52ee6ae4c}" ma:taxonomyMulti="true" ma:sspId="4aa64814-f827-41fa-8057-0fb5da987058" ma:termSetId="a50e8f86-6915-40df-8e80-3ee41e9fafc6" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="o8b80352c99244c0ae4e61fbd1c4c1b6" ma:index="16" nillable="true" ma:taxonomy="true" ma:internalName="o8b80352c99244c0ae4e61fbd1c4c1b6" ma:taxonomyFieldName="Skills_x0020__x002f__x0020_Tools" ma:displayName="Scenarios" ma:default="" ma:fieldId="{88b80352-c992-44c0-ae4e-61fbd1c4c1b6}" ma:taxonomyMulti="true" ma:sspId="4aa64814-f827-41fa-8057-0fb5da987058" ma:termSetId="440a6c62-3be0-42a9-93e7-b6d1a8cab520" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="o967d7aa727040ce921a448a49d7d2c5" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="o967d7aa727040ce921a448a49d7d2c5" ma:taxonomyFieldName="Classification" ma:displayName="Classification (for Internal only)" ma:default="" ma:fieldId="{8967d7aa-7270-40ce-921a-448a49d7d2c5}" ma:taxonomyMulti="true" ma:sspId="4aa64814-f827-41fa-8057-0fb5da987058" ma:termSetId="8b8ddd5b-b137-48e0-8ed5-e83d9587e493" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="24" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="25" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="kc0fc4540b5243a08bdce71e5c11795d" ma:index="26" nillable="true" ma:taxonomy="true" ma:internalName="kc0fc4540b5243a08bdce71e5c11795d" ma:taxonomyFieldName="Partner_x0020_Technologies" ma:displayName="Technologies" ma:default="" ma:fieldId="{4c0fc454-0b52-43a0-8bdc-e71e5c11795d}" ma:taxonomyMulti="true" ma:sspId="4aa64814-f827-41fa-8057-0fb5da987058" ma:termSetId="7f2d057d-727f-43ad-85f6-c10df3fd464b" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="30" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="31" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Flow_SignoffStatus" ma:index="32" nillable="true" ma:displayName="Sign-off status" ma:internalName="Sign_x002d_off_x0020_status">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Contributor" ma:index="33" nillable="true" ma:displayName="Contributor" ma:format="Dropdown" ma:internalName="Contributor">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="35" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="38" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="39" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6eaee64e-3edc-4652-811c-08ca3112fb23" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="15" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{0898cb8e-b6eb-429e-b3d1-e48c604af501}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="6eaee64e-3edc-4652-811c-08ca3112fb23">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="21" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="22" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="27" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B670539C-F973-45BE-9898-B45D87FF5820}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="6eaee64e-3edc-4652-811c-08ca3112fb23"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48A029B1-F269-4915-81E9-754E3C487115}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69F3F727-803A-4538-9991-F02A4FCA4F8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0b2aac62-92a3-43e0-b0c6-2d2ae436b7f7"/>
+    <ds:schemaRef ds:uri="6eaee64e-3edc-4652-811c-08ca3112fb23"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>